<commit_message>
Updated Use-case time diagram
</commit_message>
<xml_diff>
--- a/Use Cases/Use Case hours.xlsx
+++ b/Use Cases/Use Case hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>UC</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>FP</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>function</t>
+  </si>
+  <si>
+    <t>Total (Actual)</t>
+  </si>
+  <si>
+    <t>Estimation</t>
   </si>
 </sst>
 </file>
@@ -87,9 +90,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -110,8 +113,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,8 +132,13 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -167,25 +181,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
     <cellStyle name="Ergebnis" xfId="2" builtinId="25"/>
+    <cellStyle name="Gut" xfId="3" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -229,10 +260,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$2:$E$6</c:f>
+              <c:f>(Tabelle1!$E$2:$E$6,Tabelle1!$E$10:$E$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>25</c:v>
                 </c:pt>
@@ -247,16 +278,34 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$6</c:f>
+              <c:f>(Tabelle1!$F$2:$F$6,Tabelle1!$F$10:$F$15)</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5.8</c:v>
                 </c:pt>
@@ -271,6 +320,24 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>2.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,7 +356,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$10:$E$15</c:f>
+              <c:f>Tabelle1!$G$10:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -342,12 +409,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="194675840"/>
-        <c:axId val="194677376"/>
+        <c:axId val="193549440"/>
+        <c:axId val="193551360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="194675840"/>
+        <c:axId val="193549440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,12 +438,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194677376"/>
+        <c:crossAx val="193551360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194677376"/>
+        <c:axId val="193551360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +474,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194675840"/>
+        <c:crossAx val="193549440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -422,7 +488,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -432,16 +498,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>742951</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>59056</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1906</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -748,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -774,18 +840,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="G1" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -809,7 +878,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -821,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="0">B3 + C3 + D3</f>
+        <f t="shared" ref="E3:E15" si="0">B3 + C3 + D3</f>
         <v>26</v>
       </c>
       <c r="F3" s="4">
@@ -831,7 +900,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -853,7 +922,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -874,7 +943,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -886,6 +955,7 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" s="4">
@@ -894,7 +964,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -905,7 +975,8 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F7" s="4">
@@ -914,7 +985,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -926,14 +997,14 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f>B8 + C8 + D8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -945,105 +1016,217 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f>B9 + C9 + D9</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>7</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="6">
         <f>F10/H2</f>
         <v>10.258514567090685</v>
       </c>
-      <c r="F10" s="3">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="G11" s="6">
         <f>F11/H$2</f>
         <v>26.261797291752156</v>
       </c>
-      <c r="F11" s="3">
-        <v>6.4</v>
-      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="6">
-        <f t="shared" ref="E12:E15" si="1">F12/H$2</f>
-        <v>20.927369716864998</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="F12" s="3">
         <v>5.0999999999999996</v>
       </c>
+      <c r="G12" s="6">
+        <f>F12/H$2</f>
+        <v>20.927369716864998</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="6">
-        <f t="shared" si="1"/>
-        <v>20.927369716864998</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
       </c>
       <c r="F13" s="3">
         <v>5.0999999999999996</v>
       </c>
+      <c r="G13" s="6">
+        <f>F13/H$2</f>
+        <v>20.927369716864998</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="6">
-        <f t="shared" si="1"/>
-        <v>14.36192039392696</v>
+        <v>17</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
       </c>
       <c r="F14" s="3">
         <v>3.5</v>
       </c>
+      <c r="G14" s="6">
+        <f>F14/H$2</f>
+        <v>14.36192039392696</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="6">
-        <f t="shared" si="1"/>
-        <v>9.8481739844070582</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="F15" s="3">
         <v>2.4</v>
       </c>
+      <c r="G15" s="6">
+        <f>F15/H$2</f>
+        <v>9.8481739844070582</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="13.5" thickBot="1">
       <c r="B16" s="2">
-        <f xml:space="preserve"> SUM(B2:B9)</f>
-        <v>14</v>
+        <f xml:space="preserve"> SUM(B2:B15)</f>
+        <v>20</v>
       </c>
       <c r="C16" s="2">
-        <f xml:space="preserve"> SUM(C2:C9)</f>
-        <v>114</v>
+        <f xml:space="preserve"> SUM(C2:C15)</f>
+        <v>192</v>
       </c>
       <c r="D16" s="2">
-        <f xml:space="preserve"> SUM(D2:D9)</f>
-        <v>24</v>
+        <f xml:space="preserve"> SUM(D2:D15)</f>
+        <v>37</v>
       </c>
       <c r="E16" s="2">
-        <f xml:space="preserve"> SUM(E2:E9)</f>
-        <v>152</v>
-      </c>
-      <c r="F16" s="2">
+        <f xml:space="preserve"> SUM(E2:E15)</f>
+        <v>249</v>
+      </c>
+      <c r="F16" s="10">
         <f xml:space="preserve"> SUM(F2:F8)</f>
         <v>48.5</v>
       </c>
     </row>
-    <row r="17" ht="13.5" thickTop="1"/>
+    <row r="17" spans="5:6" ht="13.5" thickTop="1"/>
+    <row r="23" spans="5:6">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="5:6">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="5:6">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="5:6">
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="5:6">
+      <c r="E28" s="7"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="5:6">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="31" spans="5:6">
+      <c r="E31" s="6"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="5:6">
+      <c r="E32" s="6"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="5:6">
+      <c r="E33" s="6"/>
+      <c r="F33" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>